<commit_message>
Update deciles at national level for select years.
</commit_message>
<xml_diff>
--- a/data/National Deciles.xlsx
+++ b/data/National Deciles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simeonalder/Dropbox/Work/Research/GitHub/clusters/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7413B05D-D18D-8243-AA29-792E80D3198E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9EAC3C-D761-104B-8AD2-E5AA4C7BBF3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3060" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{24DA64D6-1545-944D-8C8D-2D0A87709E31}"/>
+    <workbookView xWindow="-32500" yWindow="2520" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{24DA64D6-1545-944D-8C8D-2D0A87709E31}"/>
   </bookViews>
   <sheets>
     <sheet name="d5_ipw" sheetId="1" r:id="rId1"/>
@@ -419,7 +419,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BE165B2-C2A7-C546-B04B-23F1CE6A8671}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:L9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -453,6 +455,12 @@
       <c r="B2">
         <v>29.7647171020507</v>
       </c>
+      <c r="C2">
+        <v>59.448459999999997</v>
+      </c>
+      <c r="D2">
+        <v>184.08670000000001</v>
+      </c>
       <c r="E2">
         <v>0.36301708221435502</v>
       </c>
@@ -467,6 +475,12 @@
       <c r="B3">
         <v>75.461418151855398</v>
       </c>
+      <c r="C3">
+        <v>131.10720000000001</v>
+      </c>
+      <c r="D3">
+        <v>414.44819999999999</v>
+      </c>
       <c r="E3">
         <v>72.963088989257798</v>
       </c>
@@ -481,6 +495,12 @@
       <c r="B4">
         <v>129.17074584960901</v>
       </c>
+      <c r="C4">
+        <v>211.38390000000001</v>
+      </c>
+      <c r="D4">
+        <v>638.78880000000004</v>
+      </c>
       <c r="E4">
         <v>172.12176513671801</v>
       </c>
@@ -495,6 +515,12 @@
       <c r="B5">
         <v>193.83598327636699</v>
       </c>
+      <c r="C5">
+        <v>296.55860000000001</v>
+      </c>
+      <c r="D5">
+        <v>913.10350000000005</v>
+      </c>
       <c r="E5">
         <v>298.21127319335898</v>
       </c>
@@ -509,6 +535,12 @@
       <c r="B6">
         <v>270.67929077148398</v>
       </c>
+      <c r="C6">
+        <v>396.00779999999997</v>
+      </c>
+      <c r="D6">
+        <v>1232.7270000000001</v>
+      </c>
       <c r="E6">
         <v>455.44244384765602</v>
       </c>
@@ -523,6 +555,12 @@
       <c r="B7">
         <v>364.66717529296801</v>
       </c>
+      <c r="C7">
+        <v>521.18100000000004</v>
+      </c>
+      <c r="D7">
+        <v>1599.23</v>
+      </c>
       <c r="E7">
         <v>650.09783935546795</v>
       </c>
@@ -537,6 +575,12 @@
       <c r="B8">
         <v>487.87493896484301</v>
       </c>
+      <c r="C8">
+        <v>696.89329999999995</v>
+      </c>
+      <c r="D8">
+        <v>2133.864</v>
+      </c>
       <c r="E8">
         <v>902.12799072265602</v>
       </c>
@@ -551,6 +595,12 @@
       <c r="B9">
         <v>675.08245849609295</v>
       </c>
+      <c r="C9">
+        <v>949.95569999999998</v>
+      </c>
+      <c r="D9">
+        <v>2839.643</v>
+      </c>
       <c r="E9">
         <v>1278.44677734375</v>
       </c>
@@ -564,6 +614,12 @@
       </c>
       <c r="B10">
         <v>1118.60705566406</v>
+      </c>
+      <c r="C10">
+        <v>1506.7429999999999</v>
+      </c>
+      <c r="D10">
+        <v>4316.973</v>
       </c>
       <c r="E10">
         <v>1952.25952148437</v>
@@ -581,7 +637,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2A85391-08B2-0149-862B-20767CF2A25D}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:L10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -615,6 +673,12 @@
       <c r="B2">
         <v>8.1767253577709198E-2</v>
       </c>
+      <c r="C2">
+        <v>8.2492700000000002E-2</v>
+      </c>
+      <c r="D2">
+        <v>7.9876900000000001E-2</v>
+      </c>
       <c r="E2">
         <v>8.0205842852592496E-2</v>
       </c>
@@ -629,6 +693,12 @@
       <c r="B3">
         <v>8.9612372219562503E-2</v>
       </c>
+      <c r="C3">
+        <v>8.9671500000000001E-2</v>
+      </c>
+      <c r="D3">
+        <v>8.7255200000000005E-2</v>
+      </c>
       <c r="E3">
         <v>8.6959674954414395E-2</v>
       </c>
@@ -643,6 +713,12 @@
       <c r="B4">
         <v>9.6178911626339E-2</v>
       </c>
+      <c r="C4">
+        <v>9.6158300000000002E-2</v>
+      </c>
+      <c r="D4">
+        <v>9.3600900000000001E-2</v>
+      </c>
       <c r="E4">
         <v>9.2915356159210205E-2</v>
       </c>
@@ -657,6 +733,12 @@
       <c r="B5">
         <v>0.102410525083541</v>
       </c>
+      <c r="C5">
+        <v>0.10227020000000001</v>
+      </c>
+      <c r="D5">
+        <v>9.9444199999999996E-2</v>
+      </c>
       <c r="E5">
         <v>9.8680883646011394E-2</v>
       </c>
@@ -671,6 +753,12 @@
       <c r="B6">
         <v>0.10958327353000601</v>
       </c>
+      <c r="C6">
+        <v>0.1091096</v>
+      </c>
+      <c r="D6">
+        <v>0.1060017</v>
+      </c>
       <c r="E6">
         <v>0.10536037385463699</v>
       </c>
@@ -685,6 +773,12 @@
       <c r="B7">
         <v>0.117934562265873</v>
       </c>
+      <c r="C7">
+        <v>0.11605500000000001</v>
+      </c>
+      <c r="D7">
+        <v>0.1146411</v>
+      </c>
       <c r="E7">
         <v>0.112819209694862</v>
       </c>
@@ -699,6 +793,12 @@
       <c r="B8">
         <v>0.13069067895412401</v>
       </c>
+      <c r="C8">
+        <v>0.12785840000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.124265</v>
+      </c>
       <c r="E8">
         <v>0.122293584048748</v>
       </c>
@@ -713,6 +813,12 @@
       <c r="B9">
         <v>0.148359775543212</v>
       </c>
+      <c r="C9">
+        <v>0.14537700000000001</v>
+      </c>
+      <c r="D9">
+        <v>0.13944980000000001</v>
+      </c>
       <c r="E9">
         <v>0.13752093911170901</v>
       </c>
@@ -726,6 +832,12 @@
       </c>
       <c r="B10">
         <v>0.185598835349082</v>
+      </c>
+      <c r="C10">
+        <v>0.18003859999999999</v>
+      </c>
+      <c r="D10">
+        <v>0.17660380000000001</v>
       </c>
       <c r="E10">
         <v>0.173840641975402</v>
@@ -743,7 +855,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5624DCF-BC0E-DF4F-9504-0BBB5267C367}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:L10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -777,6 +891,12 @@
       <c r="B2">
         <v>1.8384255468845399E-2</v>
       </c>
+      <c r="C2">
+        <v>1.8050900000000002E-2</v>
+      </c>
+      <c r="D2">
+        <v>1.8186999999999998E-2</v>
+      </c>
       <c r="E2">
         <v>1.8131608143448798E-2</v>
       </c>
@@ -791,6 +911,12 @@
       <c r="B3">
         <v>2.2118467837572101E-2</v>
       </c>
+      <c r="C3">
+        <v>2.16072E-2</v>
+      </c>
+      <c r="D3">
+        <v>2.20593E-2</v>
+      </c>
       <c r="E3">
         <v>2.1848028525710099E-2</v>
       </c>
@@ -805,6 +931,12 @@
       <c r="B4">
         <v>2.60486360639334E-2</v>
       </c>
+      <c r="C4">
+        <v>2.53187E-2</v>
+      </c>
+      <c r="D4">
+        <v>2.6312200000000001E-2</v>
+      </c>
       <c r="E4">
         <v>2.5744363665580701E-2</v>
       </c>
@@ -819,6 +951,12 @@
       <c r="B5">
         <v>3.0847886577248601E-2</v>
       </c>
+      <c r="C5">
+        <v>2.9822499999999998E-2</v>
+      </c>
+      <c r="D5">
+        <v>3.06302E-2</v>
+      </c>
       <c r="E5">
         <v>2.9964545741677302E-2</v>
       </c>
@@ -833,6 +971,12 @@
       <c r="B6">
         <v>3.6450082436203998E-2</v>
       </c>
+      <c r="C6">
+        <v>3.42318E-2</v>
+      </c>
+      <c r="D6">
+        <v>3.5998500000000003E-2</v>
+      </c>
       <c r="E6">
         <v>3.5056129097938503E-2</v>
       </c>
@@ -847,6 +991,12 @@
       <c r="B7">
         <v>4.3076049536466599E-2</v>
       </c>
+      <c r="C7">
+        <v>4.0146800000000003E-2</v>
+      </c>
+      <c r="D7">
+        <v>4.1874399999999999E-2</v>
+      </c>
       <c r="E7">
         <v>4.0926896035671199E-2</v>
       </c>
@@ -861,6 +1011,12 @@
       <c r="B8">
         <v>5.2898719906806897E-2</v>
       </c>
+      <c r="C8">
+        <v>4.8740199999999997E-2</v>
+      </c>
+      <c r="D8">
+        <v>5.0630099999999997E-2</v>
+      </c>
       <c r="E8">
         <v>4.9644846469163902E-2</v>
       </c>
@@ -875,6 +1031,12 @@
       <c r="B9">
         <v>6.8059600889682798E-2</v>
       </c>
+      <c r="C9">
+        <v>6.1541899999999997E-2</v>
+      </c>
+      <c r="D9">
+        <v>6.4598600000000006E-2</v>
+      </c>
       <c r="E9">
         <v>6.3588142395019503E-2</v>
       </c>
@@ -888,6 +1050,12 @@
       </c>
       <c r="B10">
         <v>0.103864565491676</v>
+      </c>
+      <c r="C10">
+        <v>9.3339400000000003E-2</v>
+      </c>
+      <c r="D10">
+        <v>9.8001400000000002E-2</v>
       </c>
       <c r="E10">
         <v>9.5266431570053101E-2</v>
@@ -905,7 +1073,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46AB81A5-33FD-5048-9305-250A9B03E1A0}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:L10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -939,6 +1109,12 @@
       <c r="B2">
         <v>-2.1458023693413002E-3</v>
       </c>
+      <c r="C2">
+        <v>-2.9643699999999999E-2</v>
+      </c>
+      <c r="D2">
+        <v>-3.5790200000000001E-2</v>
+      </c>
       <c r="E2">
         <v>-5.3006213158369099E-2</v>
       </c>
@@ -953,6 +1129,12 @@
       <c r="B3">
         <v>1.89966671168804E-2</v>
       </c>
+      <c r="C3">
+        <v>-7.6458000000000003E-3</v>
+      </c>
+      <c r="D3">
+        <v>-1.18421E-2</v>
+      </c>
       <c r="E3">
         <v>-3.6325700581073803E-2</v>
       </c>
@@ -967,6 +1149,12 @@
       <c r="B4">
         <v>3.3674154430627802E-2</v>
       </c>
+      <c r="C4">
+        <v>8.0356999999999998E-3</v>
+      </c>
+      <c r="D4">
+        <v>2.3622000000000001E-3</v>
+      </c>
       <c r="E4">
         <v>-2.5193441659212099E-2</v>
       </c>
@@ -981,6 +1169,12 @@
       <c r="B5">
         <v>4.6948967501521097E-2</v>
       </c>
+      <c r="C5">
+        <v>2.1319899999999999E-2</v>
+      </c>
+      <c r="D5">
+        <v>1.33112E-2</v>
+      </c>
       <c r="E5">
         <v>-1.6188587993383401E-2</v>
       </c>
@@ -995,6 +1189,12 @@
       <c r="B6">
         <v>6.1844330281019197E-2</v>
       </c>
+      <c r="C6">
+        <v>3.4453299999999999E-2</v>
+      </c>
+      <c r="D6">
+        <v>2.46228E-2</v>
+      </c>
       <c r="E6">
         <v>-7.0780203677714001E-3</v>
       </c>
@@ -1009,6 +1209,12 @@
       <c r="B7">
         <v>7.8748084604740101E-2</v>
       </c>
+      <c r="C7">
+        <v>4.92048E-2</v>
+      </c>
+      <c r="D7">
+        <v>3.7133300000000001E-2</v>
+      </c>
       <c r="E7">
         <v>4.0744701400399E-3</v>
       </c>
@@ -1023,6 +1229,12 @@
       <c r="B8">
         <v>9.7263790667056996E-2</v>
       </c>
+      <c r="C8">
+        <v>6.3814999999999997E-2</v>
+      </c>
+      <c r="D8">
+        <v>5.1940899999999998E-2</v>
+      </c>
       <c r="E8">
         <v>1.5752756968140599E-2</v>
       </c>
@@ -1037,6 +1249,12 @@
       <c r="B9">
         <v>0.125250108540058</v>
       </c>
+      <c r="C9">
+        <v>8.6200499999999999E-2</v>
+      </c>
+      <c r="D9">
+        <v>7.4449899999999999E-2</v>
+      </c>
       <c r="E9">
         <v>3.1479705125093502E-2</v>
       </c>
@@ -1050,6 +1268,12 @@
       </c>
       <c r="B10">
         <v>0.16630358994007099</v>
+      </c>
+      <c r="C10">
+        <v>0.12426760000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.1117935</v>
       </c>
       <c r="E10">
         <v>5.9343513101339299E-2</v>
@@ -1067,7 +1291,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F21313C4-71B9-C446-B53A-28A2D207F11F}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:L10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1101,6 +1327,12 @@
       <c r="B2">
         <v>-1.9619140774011602E-2</v>
       </c>
+      <c r="C2">
+        <v>-0.15363479999999999</v>
+      </c>
+      <c r="D2">
+        <v>-9.3285900000000005E-2</v>
+      </c>
       <c r="E2">
         <v>-0.193206131458282</v>
       </c>
@@ -1115,6 +1347,12 @@
       <c r="B3">
         <v>4.7575620934367201E-2</v>
       </c>
+      <c r="C3">
+        <v>-7.3532700000000006E-2</v>
+      </c>
+      <c r="D3">
+        <v>-3.2464E-2</v>
+      </c>
       <c r="E3">
         <v>-0.134210765361785</v>
       </c>
@@ -1129,6 +1367,12 @@
       <c r="B4">
         <v>8.6982160806655898E-2</v>
       </c>
+      <c r="C4">
+        <v>-2.9054400000000001E-2</v>
+      </c>
+      <c r="D4">
+        <v>4.3645999999999997E-3</v>
+      </c>
       <c r="E4">
         <v>-0.101170644164085</v>
       </c>
@@ -1143,6 +1387,12 @@
       <c r="B5">
         <v>0.120126392692327</v>
       </c>
+      <c r="C5">
+        <v>6.0108000000000002E-3</v>
+      </c>
+      <c r="D5">
+        <v>3.5472200000000002E-2</v>
+      </c>
       <c r="E5">
         <v>-7.5135443359613405E-2</v>
       </c>
@@ -1157,6 +1407,12 @@
       <c r="B6">
         <v>0.14992381632328</v>
       </c>
+      <c r="C6">
+        <v>3.5074000000000001E-2</v>
+      </c>
+      <c r="D6">
+        <v>6.1279E-2</v>
+      </c>
       <c r="E6">
         <v>-5.0849430263042401E-2</v>
       </c>
@@ -1171,6 +1427,12 @@
       <c r="B7">
         <v>0.18135825544595699</v>
       </c>
+      <c r="C7">
+        <v>6.5766599999999995E-2</v>
+      </c>
+      <c r="D7">
+        <v>9.13109E-2</v>
+      </c>
       <c r="E7">
         <v>-2.8441987000405799E-2</v>
       </c>
@@ -1185,6 +1447,12 @@
       <c r="B8">
         <v>0.21593073010444599</v>
       </c>
+      <c r="C8">
+        <v>9.5774600000000001E-2</v>
+      </c>
+      <c r="D8">
+        <v>0.1226429</v>
+      </c>
       <c r="E8">
         <v>-2.1552895195781998E-3</v>
       </c>
@@ -1199,6 +1467,12 @@
       <c r="B9">
         <v>0.263311147689819</v>
       </c>
+      <c r="C9">
+        <v>0.1356697</v>
+      </c>
+      <c r="D9">
+        <v>0.17338700000000001</v>
+      </c>
       <c r="E9">
         <v>2.9499815776944199E-2</v>
       </c>
@@ -1212,6 +1486,12 @@
       </c>
       <c r="B10">
         <v>0.34061551094055098</v>
+      </c>
+      <c r="C10">
+        <v>0.19870850000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.24338419999999999</v>
       </c>
       <c r="E10">
         <v>8.6827434599399594E-2</v>
@@ -1229,7 +1509,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FBBEFA8-4021-AD41-8B0E-9A0EBFFF56EF}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1263,6 +1545,12 @@
       <c r="B2">
         <v>-0.34891012310981701</v>
       </c>
+      <c r="C2">
+        <v>-0.60149450000000004</v>
+      </c>
+      <c r="D2">
+        <v>-0.43704409999999999</v>
+      </c>
       <c r="E2">
         <v>-0.595062315464019</v>
       </c>
@@ -1277,6 +1565,12 @@
       <c r="B3">
         <v>-0.14809043705463401</v>
       </c>
+      <c r="C3">
+        <v>-0.36643029999999999</v>
+      </c>
+      <c r="D3">
+        <v>-0.25691039999999998</v>
+      </c>
       <c r="E3">
         <v>-0.38632732629776001</v>
       </c>
@@ -1291,6 +1585,12 @@
       <c r="B4">
         <v>-5.2515350282192202E-2</v>
       </c>
+      <c r="C4">
+        <v>-0.25357809999999997</v>
+      </c>
+      <c r="D4">
+        <v>-0.15795519999999999</v>
+      </c>
       <c r="E4">
         <v>-0.28438717126846302</v>
       </c>
@@ -1305,6 +1605,12 @@
       <c r="B5">
         <v>1.2174414470791799E-2</v>
       </c>
+      <c r="C5">
+        <v>-0.19001309999999999</v>
+      </c>
+      <c r="D5">
+        <v>-8.7112499999999995E-2</v>
+      </c>
       <c r="E5">
         <v>-0.21624015271663599</v>
       </c>
@@ -1319,6 +1625,12 @@
       <c r="B6">
         <v>7.4202388525009197E-2</v>
       </c>
+      <c r="C6">
+        <v>-0.12540380000000001</v>
+      </c>
+      <c r="D6">
+        <v>-2.4244499999999999E-2</v>
+      </c>
       <c r="E6">
         <v>-0.157650306820869</v>
       </c>
@@ -1333,6 +1645,12 @@
       <c r="B7">
         <v>0.13654114305973</v>
       </c>
+      <c r="C7">
+        <v>-6.7913600000000005E-2</v>
+      </c>
+      <c r="D7">
+        <v>3.6126100000000001E-2</v>
+      </c>
       <c r="E7">
         <v>-0.10587743669748299</v>
       </c>
@@ -1347,6 +1665,12 @@
       <c r="B8">
         <v>0.20465046167373599</v>
       </c>
+      <c r="C8">
+        <v>-3.7604000000000001E-3</v>
+      </c>
+      <c r="D8">
+        <v>0.10899739999999999</v>
+      </c>
       <c r="E8">
         <v>-4.7688964754342998E-2</v>
       </c>
@@ -1361,6 +1685,12 @@
       <c r="B9">
         <v>0.30224397778510997</v>
       </c>
+      <c r="C9">
+        <v>8.6478100000000002E-2</v>
+      </c>
+      <c r="D9">
+        <v>0.2216361</v>
+      </c>
       <c r="E9">
         <v>2.9665408656001101E-2</v>
       </c>
@@ -1374,6 +1704,12 @@
       </c>
       <c r="B10">
         <v>0.49496090412139798</v>
+      </c>
+      <c r="C10">
+        <v>0.26026110000000002</v>
+      </c>
+      <c r="D10">
+        <v>0.43679820000000003</v>
       </c>
       <c r="E10">
         <v>0.18348740041255901</v>

</xml_diff>